<commit_message>
Bypass ASCII AA AB ...
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="맑은 고딕"/>
       <family val="2"/>
@@ -49,6 +49,12 @@
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="14"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="30"/>
     </font>
     <font>
       <name val="맑은 고딕"/>
@@ -173,8 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -188,15 +198,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -562,19 +581,20 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
   <cols>
-    <col width="22.296875" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="33.69921875" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="22.296875" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
+    <col width="33.69921875" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" s="4">
+    <row r="1" ht="19.5" customHeight="1" s="6">
+      <c r="B1" s="7" t="n"/>
       <c r="C1" t="inlineStr">
         <is>
           <t>damaged</t>
@@ -591,36 +611,36 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="25.5" customHeight="1" s="4">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="2" t="inlineStr">
+    <row r="2" ht="25.5" customHeight="1" s="6">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="12" t="inlineStr">
         <is>
           <t>images.png</t>
         </is>
       </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="D2" s="12" t="inlineStr">
         <is>
           <t>kid.png</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>som.png</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="25.5" customHeight="1" s="4">
-      <c r="A3" s="10" t="inlineStr">
+    <row r="3" ht="25.5" customHeight="1" s="6">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>PSNR</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
@@ -635,9 +655,9 @@
         <v>19.78924932734241</v>
       </c>
     </row>
-    <row r="4" ht="25.5" customHeight="1" s="4">
-      <c r="A4" s="11" t="n"/>
-      <c r="B4" s="3" t="inlineStr">
+    <row r="4" ht="25.5" customHeight="1" s="6">
+      <c r="A4" s="13" t="n"/>
+      <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
@@ -652,9 +672,9 @@
         <v>21.28870856671938</v>
       </c>
     </row>
-    <row r="5" ht="25.5" customHeight="1" s="4">
-      <c r="A5" s="11" t="n"/>
-      <c r="B5" s="3" t="inlineStr">
+    <row r="5" ht="25.5" customHeight="1" s="6">
+      <c r="A5" s="13" t="n"/>
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
@@ -669,9 +689,9 @@
         <v>20.79570747694748</v>
       </c>
     </row>
-    <row r="6" ht="26.25" customHeight="1" s="4">
-      <c r="A6" s="12" t="n"/>
-      <c r="B6" s="3" t="inlineStr">
+    <row r="6" ht="26.25" customHeight="1" s="6">
+      <c r="A6" s="14" t="n"/>
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
@@ -686,14 +706,16 @@
         <v>20.53669243531387</v>
       </c>
     </row>
-    <row r="7" ht="19.5" customHeight="1" s="4"/>
-    <row r="8" ht="25.5" customHeight="1" s="4">
-      <c r="A8" s="10" t="inlineStr">
+    <row r="7" ht="19.5" customHeight="1" s="6">
+      <c r="B7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="25.5" customHeight="1" s="6">
+      <c r="A8" s="8" t="inlineStr">
         <is>
           <t>SSIM</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
@@ -708,9 +730,9 @@
         <v>0.6485202433636156</v>
       </c>
     </row>
-    <row r="9" ht="25.5" customHeight="1" s="4">
-      <c r="A9" s="11" t="n"/>
-      <c r="B9" s="3" t="inlineStr">
+    <row r="9" ht="25.5" customHeight="1" s="6">
+      <c r="A9" s="13" t="n"/>
+      <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
@@ -725,9 +747,9 @@
         <v>0.6832550117653651</v>
       </c>
     </row>
-    <row r="10" ht="25.5" customHeight="1" s="4">
-      <c r="A10" s="11" t="n"/>
-      <c r="B10" s="3" t="inlineStr">
+    <row r="10" ht="25.5" customHeight="1" s="6">
+      <c r="A10" s="13" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
@@ -742,9 +764,9 @@
         <v>0.6718501949682452</v>
       </c>
     </row>
-    <row r="11" ht="26.25" customHeight="1" s="4">
-      <c r="A11" s="12" t="n"/>
-      <c r="B11" s="3" t="inlineStr">
+    <row r="11" ht="26.25" customHeight="1" s="6">
+      <c r="A11" s="14" t="n"/>
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
@@ -759,9 +781,14 @@
         <v>0.6499316388432322</v>
       </c>
     </row>
-    <row r="12" ht="19.5" customHeight="1" s="4"/>
-    <row r="13" ht="19.5" customHeight="1" s="4"/>
-    <row r="14" ht="19.5" customHeight="1" s="4">
+    <row r="12" ht="19.5" customHeight="1" s="6">
+      <c r="B12" s="7" t="n"/>
+    </row>
+    <row r="13" ht="19.5" customHeight="1" s="6">
+      <c r="B13" s="7" t="n"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" s="6">
+      <c r="B14" s="7" t="n"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>high_res</t>
@@ -773,148 +800,155 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="25.5" customHeight="1" s="4">
-      <c r="A15" s="1" t="n"/>
-      <c r="B15" s="2" t="inlineStr">
+    <row r="15" ht="25.5" customHeight="1" s="6">
+      <c r="A15" s="3" t="n"/>
+      <c r="B15" s="4" t="inlineStr">
         <is>
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C15" s="7" t="inlineStr">
+      <c r="C15" s="15" t="inlineStr">
+        <is>
+          <t>elelphant.png</t>
+        </is>
+      </c>
+      <c r="D15" s="15" t="inlineStr">
         <is>
           <t>yoshi.png</t>
         </is>
       </c>
-      <c r="D15" s="7" t="inlineStr">
-        <is>
-          <t>elelphant.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="25.5" customHeight="1" s="4">
-      <c r="A16" s="10" t="inlineStr">
+    </row>
+    <row r="16" ht="25.5" customHeight="1" s="6">
+      <c r="A16" s="8" t="inlineStr">
         <is>
           <t>PSNR</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
       </c>
       <c r="C16" t="n">
+        <v>21.05770134573583</v>
+      </c>
+      <c r="D16" t="n">
         <v>22.18728140903316</v>
       </c>
-      <c r="D16" t="n">
-        <v>21.05770134573583</v>
-      </c>
-    </row>
-    <row r="17" ht="25.5" customHeight="1" s="4">
-      <c r="A17" s="11" t="n"/>
-      <c r="B17" s="3" t="inlineStr">
+    </row>
+    <row r="17" ht="25.5" customHeight="1" s="6">
+      <c r="A17" s="13" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
       <c r="C17" t="n">
+        <v>22.40413093045892</v>
+      </c>
+      <c r="D17" t="n">
         <v>24.43339056932131</v>
       </c>
-      <c r="D17" t="n">
-        <v>22.40413093045892</v>
-      </c>
-    </row>
-    <row r="18" ht="25.5" customHeight="1" s="4">
-      <c r="A18" s="11" t="n"/>
-      <c r="B18" s="3" t="inlineStr">
+    </row>
+    <row r="18" ht="25.5" customHeight="1" s="6">
+      <c r="A18" s="13" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
       <c r="C18" t="n">
+        <v>21.86561441741668</v>
+      </c>
+      <c r="D18" t="n">
         <v>24.54475028645806</v>
       </c>
-      <c r="D18" t="n">
-        <v>21.86561441741668</v>
-      </c>
-    </row>
-    <row r="19" ht="26.25" customHeight="1" s="4">
-      <c r="A19" s="12" t="n"/>
-      <c r="B19" s="3" t="inlineStr">
+    </row>
+    <row r="19" ht="26.25" customHeight="1" s="6">
+      <c r="A19" s="14" t="n"/>
+      <c r="B19" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
       <c r="C19" t="n">
+        <v>21.65321509345508</v>
+      </c>
+      <c r="D19" t="n">
         <v>24.36872805862952</v>
       </c>
-      <c r="D19" t="n">
-        <v>21.65321509345508</v>
-      </c>
-    </row>
-    <row r="20" ht="19.5" customHeight="1" s="4"/>
-    <row r="21" ht="25.5" customHeight="1" s="4">
-      <c r="A21" s="10" t="inlineStr">
+    </row>
+    <row r="20" ht="19.5" customHeight="1" s="6">
+      <c r="B20" s="7" t="n"/>
+    </row>
+    <row r="21" ht="25.5" customHeight="1" s="6">
+      <c r="A21" s="8" t="inlineStr">
         <is>
           <t>SSIM</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
       </c>
       <c r="C21" t="n">
+        <v>0.5529713432277176</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.8684816602831141</v>
       </c>
-      <c r="D21" t="n">
-        <v>0.5529713432277176</v>
-      </c>
-    </row>
-    <row r="22" ht="25.5" customHeight="1" s="4">
-      <c r="A22" s="11" t="n"/>
-      <c r="B22" s="3" t="inlineStr">
+    </row>
+    <row r="22" ht="25.5" customHeight="1" s="6">
+      <c r="A22" s="13" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
       <c r="C22" t="n">
+        <v>0.59029945537462</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.8887026629287799</v>
       </c>
-      <c r="D22" t="n">
-        <v>0.59029945537462</v>
-      </c>
-    </row>
-    <row r="23" ht="25.5" customHeight="1" s="4">
-      <c r="A23" s="11" t="n"/>
-      <c r="B23" s="3" t="inlineStr">
+    </row>
+    <row r="23" ht="25.5" customHeight="1" s="6">
+      <c r="A23" s="13" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
       <c r="C23" t="n">
+        <v>0.5791988690138677</v>
+      </c>
+      <c r="D23" t="n">
         <v>0.884343691640277</v>
       </c>
-      <c r="D23" t="n">
-        <v>0.5791988690138677</v>
-      </c>
-    </row>
-    <row r="24" ht="19.5" customHeight="1" s="4">
-      <c r="A24" s="12" t="n"/>
-      <c r="B24" s="3" t="inlineStr">
+    </row>
+    <row r="24" ht="19.5" customHeight="1" s="6">
+      <c r="A24" s="14" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
       <c r="C24" t="n">
+        <v>0.5649646185147499</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.8531538234990826</v>
       </c>
-      <c r="D24" t="n">
-        <v>0.5649646185147499</v>
-      </c>
-    </row>
-    <row r="25" ht="19.5" customHeight="1" s="4"/>
-    <row r="26" ht="19.5" customHeight="1" s="4"/>
-    <row r="27" ht="19.5" customHeight="1" s="4">
+    </row>
+    <row r="25" ht="19.5" customHeight="1" s="6">
+      <c r="B25" s="7" t="n"/>
+    </row>
+    <row r="26" ht="19.5" customHeight="1" s="6">
+      <c r="B26" s="7" t="n"/>
+    </row>
+    <row r="27" ht="19.5" customHeight="1" s="6">
+      <c r="B27" s="7" t="n"/>
       <c r="C27" t="inlineStr">
         <is>
           <t>low_res</t>
@@ -926,143 +960,145 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="19.5" customHeight="1" s="4">
-      <c r="A28" s="1" t="n"/>
-      <c r="B28" s="2" t="inlineStr">
+    <row r="28" ht="19.5" customHeight="1" s="6">
+      <c r="A28" s="3" t="n"/>
+      <c r="B28" s="4" t="inlineStr">
         <is>
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C28" s="8" t="inlineStr">
+      <c r="C28" s="16" t="inlineStr">
+        <is>
+          <t>bear.png</t>
+        </is>
+      </c>
+      <c r="D28" s="16" t="inlineStr">
         <is>
           <t>man.png</t>
         </is>
       </c>
-      <c r="D28" s="8" t="inlineStr">
-        <is>
-          <t>bear.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="19.5" customHeight="1" s="4">
-      <c r="A29" s="10" t="inlineStr">
+    </row>
+    <row r="29" ht="19.5" customHeight="1" s="6">
+      <c r="A29" s="8" t="inlineStr">
         <is>
           <t>PSNR</t>
         </is>
       </c>
-      <c r="B29" s="3" t="inlineStr">
+      <c r="B29" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
       </c>
       <c r="C29" t="n">
+        <v>32.08783984901045</v>
+      </c>
+      <c r="D29" t="n">
         <v>34.6399640008014</v>
       </c>
-      <c r="D29" t="n">
-        <v>32.08783984901045</v>
-      </c>
-    </row>
-    <row r="30" ht="19.5" customHeight="1" s="4">
-      <c r="A30" s="11" t="n"/>
-      <c r="B30" s="3" t="inlineStr">
+    </row>
+    <row r="30" ht="19.5" customHeight="1" s="6">
+      <c r="A30" s="13" t="n"/>
+      <c r="B30" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
       <c r="C30" t="n">
+        <v>39.83857749239947</v>
+      </c>
+      <c r="D30" t="n">
         <v>42.09065224286996</v>
       </c>
-      <c r="D30" t="n">
-        <v>39.83857749239947</v>
-      </c>
-    </row>
-    <row r="31" ht="19.5" customHeight="1" s="4">
-      <c r="A31" s="11" t="n"/>
-      <c r="B31" s="3" t="inlineStr">
+    </row>
+    <row r="31" ht="19.5" customHeight="1" s="6">
+      <c r="A31" s="13" t="n"/>
+      <c r="B31" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
       <c r="C31" t="n">
+        <v>42.84569993505249</v>
+      </c>
+      <c r="D31" t="n">
         <v>45.84052077347912</v>
       </c>
-      <c r="D31" t="n">
-        <v>42.84569993505249</v>
-      </c>
-    </row>
-    <row r="32" ht="19.5" customHeight="1" s="4">
-      <c r="A32" s="12" t="n"/>
-      <c r="B32" s="3" t="inlineStr">
+    </row>
+    <row r="32" ht="19.5" customHeight="1" s="6">
+      <c r="A32" s="14" t="n"/>
+      <c r="B32" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
       <c r="C32" t="n">
+        <v>42.96417383600573</v>
+      </c>
+      <c r="D32" t="n">
         <v>46.88580966385058</v>
       </c>
-      <c r="D32" t="n">
-        <v>42.96417383600573</v>
-      </c>
-    </row>
-    <row r="33" ht="19.5" customHeight="1" s="4"/>
-    <row r="34" ht="19.5" customHeight="1" s="4">
-      <c r="A34" s="10" t="inlineStr">
+    </row>
+    <row r="33" ht="19.5" customHeight="1" s="6">
+      <c r="B33" s="7" t="n"/>
+    </row>
+    <row r="34" ht="19.5" customHeight="1" s="6">
+      <c r="A34" s="8" t="inlineStr">
         <is>
           <t>SSIM</t>
         </is>
       </c>
-      <c r="B34" s="3" t="inlineStr">
+      <c r="B34" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
       </c>
       <c r="C34" t="n">
+        <v>0.8776004899097268</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.9234198623947227</v>
       </c>
-      <c r="D34" t="n">
-        <v>0.8776004899097268</v>
-      </c>
-    </row>
-    <row r="35" ht="19.5" customHeight="1" s="4">
-      <c r="A35" s="11" t="n"/>
-      <c r="B35" s="3" t="inlineStr">
+    </row>
+    <row r="35" ht="19.5" customHeight="1" s="6">
+      <c r="A35" s="13" t="n"/>
+      <c r="B35" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
       <c r="C35" t="n">
+        <v>0.9699343460826042</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.9818988094121996</v>
       </c>
-      <c r="D35" t="n">
-        <v>0.9699343460826042</v>
-      </c>
-    </row>
-    <row r="36" ht="19.5" customHeight="1" s="4">
-      <c r="A36" s="11" t="n"/>
-      <c r="B36" s="3" t="inlineStr">
+    </row>
+    <row r="36" ht="19.5" customHeight="1" s="6">
+      <c r="A36" s="13" t="n"/>
+      <c r="B36" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
       <c r="C36" t="n">
+        <v>0.9801136147919344</v>
+      </c>
+      <c r="D36" t="n">
         <v>0.9885231471152004</v>
       </c>
-      <c r="D36" t="n">
-        <v>0.9801136147919344</v>
-      </c>
-    </row>
-    <row r="37" ht="19.5" customHeight="1" s="4">
-      <c r="A37" s="12" t="n"/>
-      <c r="B37" s="3" t="inlineStr">
+    </row>
+    <row r="37" ht="19.5" customHeight="1" s="6">
+      <c r="A37" s="14" t="n"/>
+      <c r="B37" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
       <c r="C37" t="n">
+        <v>0.9805386676558192</v>
+      </c>
+      <c r="D37" t="n">
         <v>0.9899236687075338</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.9805386676558192</v>
       </c>
     </row>
     <row r="40">
@@ -1077,31 +1113,31 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="21" customHeight="1" s="4">
-      <c r="A41" s="1" t="n"/>
-      <c r="B41" s="2" t="inlineStr">
+    <row r="41" ht="21" customHeight="1" s="6">
+      <c r="A41" s="3" t="n"/>
+      <c r="B41" s="4" t="inlineStr">
         <is>
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C41" s="9" t="inlineStr">
+      <c r="C41" s="17" t="inlineStr">
         <is>
           <t>pikachu.png</t>
         </is>
       </c>
-      <c r="D41" s="9" t="inlineStr">
+      <c r="D41" s="17" t="inlineStr">
         <is>
           <t>tree.png</t>
         </is>
       </c>
     </row>
-    <row r="42" ht="21" customHeight="1" s="4">
-      <c r="A42" s="10" t="inlineStr">
+    <row r="42" ht="21" customHeight="1" s="6">
+      <c r="A42" s="8" t="inlineStr">
         <is>
           <t>PSNR</t>
         </is>
       </c>
-      <c r="B42" s="3" t="inlineStr">
+      <c r="B42" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
@@ -1113,9 +1149,9 @@
         <v>21.46219089626999</v>
       </c>
     </row>
-    <row r="43" ht="21" customHeight="1" s="4">
-      <c r="A43" s="11" t="n"/>
-      <c r="B43" s="3" t="inlineStr">
+    <row r="43" ht="21" customHeight="1" s="6">
+      <c r="A43" s="13" t="n"/>
+      <c r="B43" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
@@ -1127,9 +1163,9 @@
         <v>23.84615234192509</v>
       </c>
     </row>
-    <row r="44" ht="21" customHeight="1" s="4">
-      <c r="A44" s="11" t="n"/>
-      <c r="B44" s="3" t="inlineStr">
+    <row r="44" ht="21" customHeight="1" s="6">
+      <c r="A44" s="13" t="n"/>
+      <c r="B44" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
@@ -1141,9 +1177,9 @@
         <v>24.00816845680683</v>
       </c>
     </row>
-    <row r="45" ht="21" customHeight="1" s="4">
-      <c r="A45" s="12" t="n"/>
-      <c r="B45" s="3" t="inlineStr">
+    <row r="45" ht="21" customHeight="1" s="6">
+      <c r="A45" s="14" t="n"/>
+      <c r="B45" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
@@ -1155,13 +1191,13 @@
         <v>24.01960888119929</v>
       </c>
     </row>
-    <row r="47" ht="21" customHeight="1" s="4">
-      <c r="A47" s="10" t="inlineStr">
+    <row r="47" ht="21" customHeight="1" s="6">
+      <c r="A47" s="8" t="inlineStr">
         <is>
           <t>SSIM</t>
         </is>
       </c>
-      <c r="B47" s="3" t="inlineStr">
+      <c r="B47" s="5" t="inlineStr">
         <is>
           <t>Nearest Neighbor</t>
         </is>
@@ -1173,9 +1209,9 @@
         <v>0.7846553035933322</v>
       </c>
     </row>
-    <row r="48" ht="21" customHeight="1" s="4">
-      <c r="A48" s="11" t="n"/>
-      <c r="B48" s="3" t="inlineStr">
+    <row r="48" ht="21" customHeight="1" s="6">
+      <c r="A48" s="13" t="n"/>
+      <c r="B48" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
@@ -1187,9 +1223,9 @@
         <v>0.8383665889268124</v>
       </c>
     </row>
-    <row r="49" ht="21" customHeight="1" s="4">
-      <c r="A49" s="11" t="n"/>
-      <c r="B49" s="3" t="inlineStr">
+    <row r="49" ht="21" customHeight="1" s="6">
+      <c r="A49" s="13" t="n"/>
+      <c r="B49" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
@@ -1201,9 +1237,9 @@
         <v>0.8351796680615702</v>
       </c>
     </row>
-    <row r="50" ht="21" customHeight="1" s="4">
-      <c r="A50" s="12" t="n"/>
-      <c r="B50" s="3" t="inlineStr">
+    <row r="50" ht="21" customHeight="1" s="6">
+      <c r="A50" s="14" t="n"/>
+      <c r="B50" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>

</xml_diff>

<commit_message>
paint max & min
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -64,7 +64,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -79,6 +79,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="3"/>
       </patternFill>
     </fill>
     <fill>
@@ -179,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -211,11 +221,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -610,6 +622,16 @@
           <t>damaged / 15</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>damaged / 15</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>damaged / 15</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="25.5" customHeight="1" s="6">
       <c r="A2" s="3" t="n"/>
@@ -620,15 +642,25 @@
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
+          <t>family.png</t>
+        </is>
+      </c>
+      <c r="D2" s="12" t="inlineStr">
+        <is>
           <t>images.png</t>
         </is>
       </c>
-      <c r="D2" s="12" t="inlineStr">
+      <c r="E2" s="12" t="inlineStr">
         <is>
           <t>kid.png</t>
         </is>
       </c>
-      <c r="E2" s="12" t="inlineStr">
+      <c r="F2" s="12" t="inlineStr">
+        <is>
+          <t>marry.png</t>
+        </is>
+      </c>
+      <c r="G2" s="12" t="inlineStr">
         <is>
           <t>som.png</t>
         </is>
@@ -645,64 +677,88 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="13" t="n">
+        <v>18.72702272791578</v>
+      </c>
+      <c r="D3" s="13" t="n">
         <v>23.92636339514132</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" s="13" t="n">
         <v>24.06194911677096</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" s="13" t="n">
+        <v>17.68388058051656</v>
+      </c>
+      <c r="G3" s="13" t="n">
         <v>18.32067128099025</v>
       </c>
     </row>
     <row r="4" ht="25.5" customHeight="1" s="6">
-      <c r="A4" s="13" t="n"/>
+      <c r="A4" s="14" t="n"/>
       <c r="B4" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="15" t="n">
+        <v>20.55932848375159</v>
+      </c>
+      <c r="D4" s="15" t="n">
         <v>25.2305021408594</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" s="15" t="n">
         <v>26.23843845769269</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" s="15" t="n">
+        <v>19.33241593667804</v>
+      </c>
+      <c r="G4" s="15" t="n">
         <v>19.72805234229667</v>
       </c>
     </row>
     <row r="5" ht="25.5" customHeight="1" s="6">
-      <c r="A5" s="13" t="n"/>
+      <c r="A5" s="14" t="n"/>
       <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
       <c r="C5" t="n">
+        <v>20.30509685497746</v>
+      </c>
+      <c r="D5" t="n">
         <v>24.77992727174584</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>25.93342514760181</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
+        <v>19.06163608668615</v>
+      </c>
+      <c r="G5" t="n">
         <v>19.28258915007475</v>
       </c>
     </row>
     <row r="6" ht="26.25" customHeight="1" s="6">
-      <c r="A6" s="14" t="n"/>
+      <c r="A6" s="16" t="n"/>
       <c r="B6" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
       <c r="C6" t="n">
+        <v>20.09614295262798</v>
+      </c>
+      <c r="D6" t="n">
         <v>24.57886448281363</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>25.71964303322285</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
+        <v>18.88761262495144</v>
+      </c>
+      <c r="G6" t="n">
         <v>19.06560490215001</v>
       </c>
     </row>
@@ -720,64 +776,88 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="13" t="n">
+        <v>0.5207279125965014</v>
+      </c>
+      <c r="D8" s="13" t="n">
         <v>0.6075442736222051</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" s="13" t="n">
         <v>0.7828164420241289</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" s="13" t="n">
+        <v>0.4806374191604903</v>
+      </c>
+      <c r="G8" s="13" t="n">
         <v>0.5437072685746848</v>
       </c>
     </row>
     <row r="9" ht="25.5" customHeight="1" s="6">
-      <c r="A9" s="13" t="n"/>
+      <c r="A9" s="14" t="n"/>
       <c r="B9" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="15" t="n">
+        <v>0.593940833185831</v>
+      </c>
+      <c r="D9" s="15" t="n">
         <v>0.6681027314701836</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" s="15" t="n">
         <v>0.8403135876897583</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" s="15" t="n">
+        <v>0.5508381181938732</v>
+      </c>
+      <c r="G9" s="15" t="n">
         <v>0.5947867128619063</v>
       </c>
     </row>
     <row r="10" ht="25.5" customHeight="1" s="6">
-      <c r="A10" s="13" t="n"/>
+      <c r="A10" s="14" t="n"/>
       <c r="B10" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
       <c r="C10" t="n">
+        <v>0.5807633801972012</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.6567860866040037</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.8332756753608379</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
+        <v>0.5380352731172979</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.5793715295755107</v>
       </c>
     </row>
     <row r="11" ht="26.25" customHeight="1" s="6">
-      <c r="A11" s="14" t="n"/>
+      <c r="A11" s="16" t="n"/>
       <c r="B11" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
       <c r="C11" t="n">
+        <v>0.5590462774189922</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.643750231712633</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0.8210952913144416</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
+        <v>0.5185573174882072</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.5571797105868965</v>
       </c>
     </row>
@@ -809,6 +889,11 @@
           <t>high_res / 15</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>high_res / 15</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="25.5" customHeight="1" s="6">
       <c r="A15" s="3" t="n"/>
@@ -817,22 +902,27 @@
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C15" s="15" t="inlineStr">
+      <c r="C15" s="17" t="inlineStr">
         <is>
           <t>bird.png</t>
         </is>
       </c>
-      <c r="D15" s="15" t="inlineStr">
+      <c r="D15" s="17" t="inlineStr">
         <is>
           <t>elelphant.png</t>
         </is>
       </c>
-      <c r="E15" s="15" t="inlineStr">
+      <c r="E15" s="17" t="inlineStr">
+        <is>
+          <t>field.png</t>
+        </is>
+      </c>
+      <c r="F15" s="17" t="inlineStr">
         <is>
           <t>water.png</t>
         </is>
       </c>
-      <c r="F15" s="15" t="inlineStr">
+      <c r="G15" s="17" t="inlineStr">
         <is>
           <t>yoshi.png</t>
         </is>
@@ -849,41 +939,47 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="13" t="n">
         <v>29.79702444375747</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="13" t="n">
         <v>20.33668350233375</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="13" t="n">
+        <v>19.76267950534896</v>
+      </c>
+      <c r="F16" s="13" t="n">
         <v>22.64643209512656</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" s="13" t="n">
         <v>19.51690542402421</v>
       </c>
     </row>
     <row r="17" ht="25.5" customHeight="1" s="6">
-      <c r="A17" s="13" t="n"/>
+      <c r="A17" s="14" t="n"/>
       <c r="B17" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="15" t="n">
         <v>31.87549340974631</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="15" t="n">
         <v>21.58626816235147</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="15" t="n">
+        <v>21.0649889105438</v>
+      </c>
+      <c r="F17" s="15" t="n">
         <v>23.86744155311609</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>21.76058903298207</v>
       </c>
     </row>
     <row r="18" ht="25.5" customHeight="1" s="6">
-      <c r="A18" s="13" t="n"/>
+      <c r="A18" s="14" t="n"/>
       <c r="B18" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
@@ -896,14 +992,17 @@
         <v>21.20893333404922</v>
       </c>
       <c r="E18" t="n">
+        <v>20.84708854037841</v>
+      </c>
+      <c r="F18" t="n">
         <v>23.45145508091065</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" s="15" t="n">
         <v>21.93521364411928</v>
       </c>
     </row>
     <row r="19" ht="26.25" customHeight="1" s="6">
-      <c r="A19" s="14" t="n"/>
+      <c r="A19" s="16" t="n"/>
       <c r="B19" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
@@ -916,9 +1015,12 @@
         <v>21.05384609543152</v>
       </c>
       <c r="E19" t="n">
+        <v>20.68320761235014</v>
+      </c>
+      <c r="F19" t="n">
         <v>23.21451170423998</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>21.85740011982916</v>
       </c>
     </row>
@@ -936,21 +1038,24 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="13" t="n">
         <v>0.9297294479068317</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="13" t="n">
         <v>0.468237542278865</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="13" t="n">
+        <v>0.6220931843304346</v>
+      </c>
+      <c r="F21" s="13" t="n">
         <v>0.5798681931620625</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>0.7834676151154504</v>
       </c>
     </row>
     <row r="22" ht="25.5" customHeight="1" s="6">
-      <c r="A22" s="13" t="n"/>
+      <c r="A22" s="14" t="n"/>
       <c r="B22" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
@@ -959,38 +1064,44 @@
       <c r="C22" t="n">
         <v>0.9559037338313137</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="15" t="n">
         <v>0.5192287376066872</v>
       </c>
       <c r="E22" t="n">
+        <v>0.6645829324232028</v>
+      </c>
+      <c r="F22" s="15" t="n">
         <v>0.6342269231159152</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" s="15" t="n">
         <v>0.8181389371542295</v>
       </c>
     </row>
     <row r="23" ht="25.5" customHeight="1" s="6">
-      <c r="A23" s="13" t="n"/>
+      <c r="A23" s="14" t="n"/>
       <c r="B23" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="15" t="n">
         <v>0.9571114066253193</v>
       </c>
       <c r="D23" t="n">
         <v>0.507529922948876</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" s="15" t="n">
+        <v>0.6664123890754344</v>
+      </c>
+      <c r="F23" t="n">
         <v>0.6266431131173542</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>0.8079883687904585</v>
       </c>
     </row>
     <row r="24" ht="19.5" customHeight="1" s="6">
-      <c r="A24" s="14" t="n"/>
+      <c r="A24" s="16" t="n"/>
       <c r="B24" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
@@ -1003,9 +1114,12 @@
         <v>0.4963430525203361</v>
       </c>
       <c r="E24" t="n">
+        <v>0.6590362666832175</v>
+      </c>
+      <c r="F24" t="n">
         <v>0.6155594439617312</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" s="13" t="n">
         <v>0.7661920629065585</v>
       </c>
     </row>
@@ -1035,12 +1149,12 @@
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C28" s="16" t="inlineStr">
+      <c r="C28" s="18" t="inlineStr">
         <is>
           <t>bear.png</t>
         </is>
       </c>
-      <c r="D28" s="16" t="inlineStr">
+      <c r="D28" s="18" t="inlineStr">
         <is>
           <t>man.png</t>
         </is>
@@ -1057,15 +1171,15 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" s="13" t="n">
         <v>28.77891269925218</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29" s="13" t="n">
         <v>30.20098261151398</v>
       </c>
     </row>
     <row r="30" ht="19.5" customHeight="1" s="6">
-      <c r="A30" s="13" t="n"/>
+      <c r="A30" s="14" t="n"/>
       <c r="B30" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
@@ -1079,7 +1193,7 @@
       </c>
     </row>
     <row r="31" ht="19.5" customHeight="1" s="6">
-      <c r="A31" s="13" t="n"/>
+      <c r="A31" s="14" t="n"/>
       <c r="B31" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
@@ -1093,16 +1207,16 @@
       </c>
     </row>
     <row r="32" ht="19.5" customHeight="1" s="6">
-      <c r="A32" s="14" t="n"/>
+      <c r="A32" s="16" t="n"/>
       <c r="B32" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="15" t="n">
         <v>34.72650061785436</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32" s="15" t="n">
         <v>37.40432538930059</v>
       </c>
     </row>
@@ -1120,15 +1234,15 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" s="13" t="n">
         <v>0.7689866038485912</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="13" t="n">
         <v>0.8202449007268093</v>
       </c>
     </row>
     <row r="35" ht="19.5" customHeight="1" s="6">
-      <c r="A35" s="13" t="n"/>
+      <c r="A35" s="14" t="n"/>
       <c r="B35" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
@@ -1142,7 +1256,7 @@
       </c>
     </row>
     <row r="36" ht="19.5" customHeight="1" s="6">
-      <c r="A36" s="13" t="n"/>
+      <c r="A36" s="14" t="n"/>
       <c r="B36" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
@@ -1156,16 +1270,16 @@
       </c>
     </row>
     <row r="37" ht="19.5" customHeight="1" s="6">
-      <c r="A37" s="14" t="n"/>
+      <c r="A37" s="16" t="n"/>
       <c r="B37" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" s="15" t="n">
         <v>0.9121123134507707</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37" s="15" t="n">
         <v>0.945070769218908</v>
       </c>
     </row>
@@ -1223,47 +1337,47 @@
           <t>INTERPOLATION METHODS</t>
         </is>
       </c>
-      <c r="C41" s="17" t="inlineStr">
+      <c r="C41" s="19" t="inlineStr">
         <is>
           <t>axolotl.png</t>
         </is>
       </c>
-      <c r="D41" s="17" t="inlineStr">
+      <c r="D41" s="19" t="inlineStr">
         <is>
           <t>breakfast.png</t>
         </is>
       </c>
-      <c r="E41" s="17" t="inlineStr">
+      <c r="E41" s="19" t="inlineStr">
         <is>
           <t>cliff.png</t>
         </is>
       </c>
-      <c r="F41" s="17" t="inlineStr">
+      <c r="F41" s="19" t="inlineStr">
         <is>
           <t>gun.png</t>
         </is>
       </c>
-      <c r="G41" s="17" t="inlineStr">
+      <c r="G41" s="19" t="inlineStr">
         <is>
           <t>knight.png</t>
         </is>
       </c>
-      <c r="H41" s="17" t="inlineStr">
+      <c r="H41" s="19" t="inlineStr">
         <is>
           <t>pikachu.png</t>
         </is>
       </c>
-      <c r="I41" s="17" t="inlineStr">
+      <c r="I41" s="19" t="inlineStr">
         <is>
           <t>pizza.png</t>
         </is>
       </c>
-      <c r="J41" s="17" t="inlineStr">
+      <c r="J41" s="19" t="inlineStr">
         <is>
           <t>tree.png</t>
         </is>
       </c>
-      <c r="K41" s="17" t="inlineStr">
+      <c r="K41" s="19" t="inlineStr">
         <is>
           <t>wizzard.png</t>
         </is>
@@ -1280,71 +1394,71 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" s="13" t="n">
         <v>22.57125106555887</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42" s="13" t="n">
         <v>24.92943639268828</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" s="13" t="n">
         <v>32.42433408242604</v>
       </c>
-      <c r="F42" t="n">
+      <c r="F42" s="13" t="n">
         <v>24.4538847987094</v>
       </c>
-      <c r="G42" t="n">
+      <c r="G42" s="13" t="n">
         <v>22.97591850088856</v>
       </c>
-      <c r="H42" t="n">
+      <c r="H42" s="13" t="n">
         <v>13.04423328477438</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I42" s="13" t="n">
         <v>17.77389078245491</v>
       </c>
-      <c r="J42" t="n">
+      <c r="J42" s="13" t="n">
         <v>18.97185344271182</v>
       </c>
-      <c r="K42" t="n">
+      <c r="K42" s="13" t="n">
         <v>21.19825391313464</v>
       </c>
     </row>
     <row r="43" ht="21" customHeight="1" s="6">
-      <c r="A43" s="13" t="n"/>
+      <c r="A43" s="14" t="n"/>
       <c r="B43" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" s="15" t="n">
         <v>24.48134435777748</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43" s="15" t="n">
         <v>26.70519867613292</v>
       </c>
       <c r="E43" t="n">
         <v>32.54599121839482</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F43" s="15" t="n">
         <v>26.37345053767995</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G43" s="15" t="n">
         <v>24.80422631522724</v>
       </c>
-      <c r="H43" t="n">
+      <c r="H43" s="15" t="n">
         <v>14.66275042398977</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I43" s="15" t="n">
         <v>19.38367542722527</v>
       </c>
-      <c r="J43" t="n">
+      <c r="J43" s="15" t="n">
         <v>20.95634460844059</v>
       </c>
-      <c r="K43" t="n">
+      <c r="K43" s="15" t="n">
         <v>22.97404183347038</v>
       </c>
     </row>
     <row r="44" ht="21" customHeight="1" s="6">
-      <c r="A44" s="13" t="n"/>
+      <c r="A44" s="14" t="n"/>
       <c r="B44" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
@@ -1379,7 +1493,7 @@
       </c>
     </row>
     <row r="45" ht="21" customHeight="1" s="6">
-      <c r="A45" s="14" t="n"/>
+      <c r="A45" s="16" t="n"/>
       <c r="B45" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
@@ -1391,7 +1505,7 @@
       <c r="D45" t="n">
         <v>26.31560180921333</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45" s="15" t="n">
         <v>33.23097112402589</v>
       </c>
       <c r="F45" t="n">
@@ -1424,36 +1538,36 @@
           <t>Nearest Neighbor</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" s="15" t="n">
         <v>0.8972020565176916</v>
       </c>
       <c r="D47" t="n">
         <v>0.8582853080027615</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E47" s="13" t="n">
         <v>0.9069548030564748</v>
       </c>
-      <c r="F47" t="n">
+      <c r="F47" s="13" t="n">
         <v>0.8194310860942272</v>
       </c>
       <c r="G47" t="n">
         <v>0.8824249502406394</v>
       </c>
-      <c r="H47" t="n">
+      <c r="H47" s="15" t="n">
         <v>0.6889045099324446</v>
       </c>
-      <c r="I47" t="n">
+      <c r="I47" s="13" t="n">
         <v>0.6489755502869424</v>
       </c>
-      <c r="J47" t="n">
+      <c r="J47" s="13" t="n">
         <v>0.6821725008323676</v>
       </c>
-      <c r="K47" t="n">
+      <c r="K47" s="15" t="n">
         <v>0.8383062632613445</v>
       </c>
     </row>
     <row r="48" ht="21" customHeight="1" s="6">
-      <c r="A48" s="13" t="n"/>
+      <c r="A48" s="14" t="n"/>
       <c r="B48" s="5" t="inlineStr">
         <is>
           <t>Bilinear</t>
@@ -1462,25 +1576,25 @@
       <c r="C48" t="n">
         <v>0.8925856623537753</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48" s="15" t="n">
         <v>0.8758109260385373</v>
       </c>
       <c r="E48" t="n">
         <v>0.9074028354713159</v>
       </c>
-      <c r="F48" t="n">
+      <c r="F48" s="15" t="n">
         <v>0.844014377093217</v>
       </c>
-      <c r="G48" t="n">
+      <c r="G48" s="15" t="n">
         <v>0.8945322493383068</v>
       </c>
       <c r="H48" t="n">
         <v>0.6770613859104637</v>
       </c>
-      <c r="I48" t="n">
+      <c r="I48" s="15" t="n">
         <v>0.7026394593509345</v>
       </c>
-      <c r="J48" t="n">
+      <c r="J48" s="15" t="n">
         <v>0.7290468172091509</v>
       </c>
       <c r="K48" t="n">
@@ -1488,7 +1602,7 @@
       </c>
     </row>
     <row r="49" ht="21" customHeight="1" s="6">
-      <c r="A49" s="13" t="n"/>
+      <c r="A49" s="14" t="n"/>
       <c r="B49" s="5" t="inlineStr">
         <is>
           <t>Bicubic</t>
@@ -1500,7 +1614,7 @@
       <c r="D49" t="n">
         <v>0.8626969097186971</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49" s="15" t="n">
         <v>0.9100348812649616</v>
       </c>
       <c r="F49" t="n">
@@ -1523,16 +1637,16 @@
       </c>
     </row>
     <row r="50" ht="21" customHeight="1" s="6">
-      <c r="A50" s="14" t="n"/>
+      <c r="A50" s="16" t="n"/>
       <c r="B50" s="5" t="inlineStr">
         <is>
           <t>Lanczos</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" s="13" t="n">
         <v>0.8522033478410863</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50" s="13" t="n">
         <v>0.8461967591416126</v>
       </c>
       <c r="E50" t="n">
@@ -1541,10 +1655,10 @@
       <c r="F50" t="n">
         <v>0.8208673806897647</v>
       </c>
-      <c r="G50" t="n">
+      <c r="G50" s="13" t="n">
         <v>0.8753236324658685</v>
       </c>
-      <c r="H50" t="n">
+      <c r="H50" s="13" t="n">
         <v>0.6057841822753253</v>
       </c>
       <c r="I50" t="n">
@@ -1553,7 +1667,7 @@
       <c r="J50" t="n">
         <v>0.695487805303713</v>
       </c>
-      <c r="K50" t="n">
+      <c r="K50" s="13" t="n">
         <v>0.797295842732928</v>
       </c>
     </row>

</xml_diff>